<commit_message>
Beginning NFL regular season analysis
</commit_message>
<xml_diff>
--- a/CFB_and_NFL_Predictions_2024-25/NFL/regular_season.xlsx
+++ b/CFB_and_NFL_Predictions_2024-25/NFL/regular_season.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mridd\Desktop\CFB-and-NFL-Prediction-Analysis\CFB_and_NFL_Predictions_2024-25\NFL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2684FB3C-FC4F-467E-AC7D-EBAE6C9BD150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC41DE02-B8B3-49EC-871F-71D82F551A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{12A6FA16-5435-461D-8CAB-650A16FC83FE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{12A6FA16-5435-461D-8CAB-650A16FC83FE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="regular_season" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="93">
   <si>
     <t>Month</t>
   </si>
@@ -215,9 +215,6 @@
     <t>OUTRO</t>
   </si>
   <si>
-    <t>Division</t>
-  </si>
-  <si>
     <t>AFC South</t>
   </si>
   <si>
@@ -312,6 +309,12 @@
   </si>
   <si>
     <t>LDFS</t>
+  </si>
+  <si>
+    <t>Away Division</t>
+  </si>
+  <si>
+    <t>Home Division</t>
   </si>
 </sst>
 </file>
@@ -699,8 +702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA5F103D-B6A1-4E63-94B2-E1BB9111D4E9}">
   <dimension ref="A1:J149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="A142" sqref="A142"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,9 +712,9 @@
     <col min="2" max="2" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.109375" style="1"/>
     <col min="4" max="4" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -730,13 +733,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>27</v>
@@ -762,13 +765,13 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>28</v>
@@ -794,13 +797,13 @@
         <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>29</v>
@@ -826,13 +829,13 @@
         <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>30</v>
@@ -858,13 +861,13 @@
         <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>31</v>
@@ -890,13 +893,13 @@
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>32</v>
@@ -922,13 +925,13 @@
         <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>33</v>
@@ -954,13 +957,13 @@
         <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>37</v>
@@ -986,13 +989,13 @@
         <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>40</v>
@@ -1018,13 +1021,13 @@
         <v>41</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>43</v>
@@ -1050,13 +1053,13 @@
         <v>44</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>46</v>
@@ -1082,13 +1085,13 @@
         <v>47</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>49</v>
@@ -1114,13 +1117,13 @@
         <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>51</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>32</v>
@@ -1146,13 +1149,13 @@
         <v>52</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>40</v>
@@ -1178,13 +1181,13 @@
         <v>54</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>37</v>
@@ -1210,13 +1213,13 @@
         <v>56</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>57</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>58</v>
@@ -1242,13 +1245,13 @@
         <v>36</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>29</v>
@@ -1274,13 +1277,13 @@
         <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>32</v>
@@ -1306,13 +1309,13 @@
         <v>19</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>37</v>
@@ -1338,13 +1341,13 @@
         <v>41</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>57</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>31</v>
@@ -1370,13 +1373,13 @@
         <v>17</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>30</v>
@@ -1399,19 +1402,19 @@
         <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1425,19 +1428,19 @@
         <v>10</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>14</v>
@@ -1460,13 +1463,13 @@
         <v>55</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>46</v>
@@ -1492,13 +1495,13 @@
         <v>34</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>37</v>
@@ -1524,13 +1527,13 @@
         <v>45</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>43</v>
@@ -1556,16 +1559,16 @@
         <v>13</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>14</v>
@@ -1588,16 +1591,16 @@
         <v>50</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>14</v>
@@ -1620,13 +1623,13 @@
         <v>21</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>28</v>
@@ -1652,16 +1655,16 @@
         <v>35</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>20</v>
@@ -1684,13 +1687,13 @@
         <v>51</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>28</v>
@@ -1716,13 +1719,13 @@
         <v>44</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>29</v>
@@ -1748,16 +1751,16 @@
         <v>55</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>14</v>
@@ -1780,13 +1783,13 @@
         <v>22</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>37</v>
@@ -1812,16 +1815,16 @@
         <v>52</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>14</v>
@@ -1844,13 +1847,13 @@
         <v>25</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>32</v>
@@ -1876,13 +1879,13 @@
         <v>54</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>33</v>
@@ -1908,16 +1911,16 @@
         <v>42</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>14</v>
@@ -1940,16 +1943,16 @@
         <v>17</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>20</v>
@@ -1972,16 +1975,16 @@
         <v>53</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>20</v>
@@ -2004,16 +2007,16 @@
         <v>57</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>20</v>
@@ -2036,13 +2039,13 @@
         <v>23</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>37</v>
@@ -2068,16 +2071,16 @@
         <v>12</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>14</v>
@@ -2097,16 +2100,16 @@
         <v>12</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>28</v>
@@ -2132,13 +2135,13 @@
         <v>55</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>31</v>
@@ -2164,13 +2167,13 @@
         <v>50</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>37</v>
@@ -2196,13 +2199,13 @@
         <v>26</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>29</v>
@@ -2228,16 +2231,16 @@
         <v>56</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>14</v>
@@ -2260,16 +2263,16 @@
         <v>16</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>20</v>
@@ -2292,13 +2295,13 @@
         <v>57</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>30</v>
@@ -2324,13 +2327,13 @@
         <v>34</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>37</v>
@@ -2356,13 +2359,13 @@
         <v>41</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>43</v>
@@ -2385,19 +2388,19 @@
         <v>12</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>51</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>20</v>
@@ -2420,16 +2423,16 @@
         <v>48</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>20</v>
@@ -2452,13 +2455,13 @@
         <v>45</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>46</v>
@@ -2484,16 +2487,16 @@
         <v>42</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>14</v>
@@ -2516,13 +2519,13 @@
         <v>47</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>28</v>
@@ -2548,16 +2551,16 @@
         <v>36</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>20</v>
@@ -2580,13 +2583,13 @@
         <v>21</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>51</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>29</v>
@@ -2600,10 +2603,10 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C60" s="1">
         <v>13</v>
@@ -2612,13 +2615,13 @@
         <v>22</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>57</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>37</v>
@@ -2632,7 +2635,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>10</v>
@@ -2644,13 +2647,13 @@
         <v>24</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>30</v>
@@ -2664,7 +2667,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>10</v>
@@ -2673,19 +2676,19 @@
         <v>13</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>20</v>
@@ -2696,7 +2699,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>10</v>
@@ -2708,16 +2711,16 @@
         <v>48</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>20</v>
@@ -2728,7 +2731,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>10</v>
@@ -2740,16 +2743,16 @@
         <v>54</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>20</v>
@@ -2760,7 +2763,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>10</v>
@@ -2772,16 +2775,16 @@
         <v>53</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>14</v>
@@ -2792,7 +2795,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>10</v>
@@ -2804,16 +2807,16 @@
         <v>34</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>14</v>
@@ -2824,7 +2827,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>10</v>
@@ -2836,13 +2839,13 @@
         <v>12</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>37</v>
@@ -2856,7 +2859,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>10</v>
@@ -2868,16 +2871,16 @@
         <v>52</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>14</v>
@@ -2888,7 +2891,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>10</v>
@@ -2900,13 +2903,13 @@
         <v>56</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>31</v>
@@ -2920,7 +2923,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>10</v>
@@ -2932,13 +2935,13 @@
         <v>45</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>46</v>
@@ -2952,7 +2955,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>10</v>
@@ -2961,16 +2964,16 @@
         <v>13</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>37</v>
@@ -2984,7 +2987,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>11</v>
@@ -2996,13 +2999,13 @@
         <v>25</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>43</v>
@@ -3016,7 +3019,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>9</v>
@@ -3028,13 +3031,13 @@
         <v>51</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>28</v>
@@ -3048,7 +3051,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>10</v>
@@ -3060,16 +3063,16 @@
         <v>44</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>20</v>
@@ -3080,7 +3083,7 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>10</v>
@@ -3092,13 +3095,13 @@
         <v>13</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>37</v>
@@ -3112,7 +3115,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>10</v>
@@ -3124,13 +3127,13 @@
         <v>17</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>30</v>
@@ -3144,7 +3147,7 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>10</v>
@@ -3156,13 +3159,13 @@
         <v>38</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>31</v>
@@ -3176,7 +3179,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>10</v>
@@ -3188,13 +3191,13 @@
         <v>39</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>29</v>
@@ -3208,7 +3211,7 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>10</v>
@@ -3220,13 +3223,13 @@
         <v>25</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>43</v>
@@ -3240,7 +3243,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>10</v>
@@ -3252,16 +3255,16 @@
         <v>22</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>20</v>
@@ -3272,7 +3275,7 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>10</v>
@@ -3284,13 +3287,13 @@
         <v>53</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>37</v>
@@ -3304,7 +3307,7 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>10</v>
@@ -3316,13 +3319,13 @@
         <v>19</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>46</v>
@@ -3336,7 +3339,7 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>10</v>
@@ -3348,13 +3351,13 @@
         <v>47</v>
       </c>
       <c r="E83" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>37</v>
@@ -3368,7 +3371,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>10</v>
@@ -3380,16 +3383,16 @@
         <v>24</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>57</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>14</v>
@@ -3400,7 +3403,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>11</v>
@@ -3412,16 +3415,16 @@
         <v>23</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>14</v>
@@ -3432,7 +3435,7 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>9</v>
@@ -3444,13 +3447,13 @@
         <v>52</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>33</v>
@@ -3464,7 +3467,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>10</v>
@@ -3476,13 +3479,13 @@
         <v>57</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>29</v>
@@ -3496,7 +3499,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>10</v>
@@ -3508,13 +3511,13 @@
         <v>23</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>28</v>
@@ -3528,7 +3531,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>10</v>
@@ -3540,13 +3543,13 @@
         <v>35</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>37</v>
@@ -3560,7 +3563,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>10</v>
@@ -3572,13 +3575,13 @@
         <v>42</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>30</v>
@@ -3592,7 +3595,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>10</v>
@@ -3604,16 +3607,16 @@
         <v>16</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>20</v>
@@ -3624,7 +3627,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>10</v>
@@ -3636,13 +3639,13 @@
         <v>13</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>37</v>
@@ -3656,7 +3659,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>10</v>
@@ -3668,13 +3671,13 @@
         <v>21</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>43</v>
@@ -3688,7 +3691,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>10</v>
@@ -3700,16 +3703,16 @@
         <v>54</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>20</v>
@@ -3720,7 +3723,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>10</v>
@@ -3732,13 +3735,13 @@
         <v>19</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>32</v>
@@ -3752,7 +3755,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>10</v>
@@ -3761,16 +3764,16 @@
         <v>15</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H96" s="1" t="s">
         <v>46</v>
@@ -3784,7 +3787,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>10</v>
@@ -3796,13 +3799,13 @@
         <v>26</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>31</v>
@@ -3816,7 +3819,7 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>10</v>
@@ -3828,16 +3831,16 @@
         <v>56</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>14</v>
@@ -3848,7 +3851,7 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>10</v>
@@ -3860,16 +3863,16 @@
         <v>51</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>14</v>
@@ -3880,7 +3883,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>11</v>
@@ -3892,16 +3895,16 @@
         <v>47</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>20</v>
@@ -3912,7 +3915,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>11</v>
@@ -3924,16 +3927,16 @@
         <v>17</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>14</v>
@@ -3944,7 +3947,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>9</v>
@@ -3956,16 +3959,16 @@
         <v>41</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>14</v>
@@ -3976,10 +3979,10 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C103" s="1">
         <v>16</v>
@@ -3988,13 +3991,13 @@
         <v>12</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>57</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>28</v>
@@ -4008,25 +4011,25 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C104" s="1">
         <v>16</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H104" s="1" t="s">
         <v>33</v>
@@ -4040,7 +4043,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>10</v>
@@ -4052,13 +4055,13 @@
         <v>36</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>29</v>
@@ -4072,7 +4075,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>10</v>
@@ -4084,13 +4087,13 @@
         <v>26</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>37</v>
@@ -4104,7 +4107,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>10</v>
@@ -4116,13 +4119,13 @@
         <v>50</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>37</v>
@@ -4136,7 +4139,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>10</v>
@@ -4148,13 +4151,13 @@
         <v>25</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>31</v>
@@ -4168,7 +4171,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>10</v>
@@ -4180,13 +4183,13 @@
         <v>34</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>32</v>
@@ -4200,7 +4203,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>10</v>
@@ -4212,13 +4215,13 @@
         <v>52</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>30</v>
@@ -4232,7 +4235,7 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>10</v>
@@ -4244,16 +4247,16 @@
         <v>45</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>14</v>
@@ -4264,7 +4267,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>10</v>
@@ -4276,16 +4279,16 @@
         <v>48</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F112" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>14</v>
@@ -4296,7 +4299,7 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>10</v>
@@ -4308,16 +4311,16 @@
         <v>55</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F113" s="1" t="s">
         <v>53</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>14</v>
@@ -4328,7 +4331,7 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>10</v>
@@ -4340,13 +4343,13 @@
         <v>44</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>37</v>
@@ -4360,7 +4363,7 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>10</v>
@@ -4369,16 +4372,16 @@
         <v>16</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>43</v>
@@ -4392,7 +4395,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>10</v>
@@ -4404,13 +4407,13 @@
         <v>56</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F116" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>46</v>
@@ -4424,7 +4427,7 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>11</v>
@@ -4436,13 +4439,13 @@
         <v>38</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F117" s="1" t="s">
         <v>51</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>28</v>
@@ -4456,10 +4459,10 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C118" s="1">
         <v>17</v>
@@ -4468,16 +4471,16 @@
         <v>57</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I118" s="1" t="s">
         <v>20</v>
@@ -4488,10 +4491,10 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C119" s="1">
         <v>17</v>
@@ -4500,13 +4503,13 @@
         <v>42</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>29</v>
@@ -4520,7 +4523,7 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>9</v>
@@ -4532,16 +4535,16 @@
         <v>53</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>47</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I120" s="1" t="s">
         <v>20</v>
@@ -4552,10 +4555,10 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C121" s="1">
         <v>17</v>
@@ -4564,13 +4567,13 @@
         <v>24</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>37</v>
@@ -4584,10 +4587,10 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C122" s="1">
         <v>17</v>
@@ -4596,13 +4599,13 @@
         <v>41</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>32</v>
@@ -4616,10 +4619,10 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C123" s="1">
         <v>17</v>
@@ -4628,13 +4631,13 @@
         <v>48</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>28</v>
@@ -4648,7 +4651,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>10</v>
@@ -4660,13 +4663,13 @@
         <v>13</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F124" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H124" s="1" t="s">
         <v>37</v>
@@ -4680,7 +4683,7 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>10</v>
@@ -4692,16 +4695,16 @@
         <v>22</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F125" s="1" t="s">
         <v>38</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I125" s="1" t="s">
         <v>20</v>
@@ -4712,7 +4715,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>10</v>
@@ -4724,13 +4727,13 @@
         <v>54</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F126" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H126" s="1" t="s">
         <v>33</v>
@@ -4744,7 +4747,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>10</v>
@@ -4756,13 +4759,13 @@
         <v>16</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F127" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>30</v>
@@ -4776,7 +4779,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>10</v>
@@ -4788,13 +4791,13 @@
         <v>39</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H128" s="1" t="s">
         <v>37</v>
@@ -4808,7 +4811,7 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>10</v>
@@ -4820,16 +4823,16 @@
         <v>34</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>44</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I129" s="1" t="s">
         <v>20</v>
@@ -4840,7 +4843,7 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>10</v>
@@ -4852,16 +4855,16 @@
         <v>21</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I130" s="1" t="s">
         <v>14</v>
@@ -4872,7 +4875,7 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>10</v>
@@ -4884,13 +4887,13 @@
         <v>51</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F131" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H131" s="1" t="s">
         <v>46</v>
@@ -4904,7 +4907,7 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>10</v>
@@ -4916,13 +4919,13 @@
         <v>17</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F132" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H132" s="1" t="s">
         <v>31</v>
@@ -4936,7 +4939,7 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>11</v>
@@ -4948,13 +4951,13 @@
         <v>50</v>
       </c>
       <c r="E133" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G133" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G133" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H133" s="1" t="s">
         <v>43</v>
@@ -4968,10 +4971,10 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C134" s="1">
         <v>18</v>
@@ -4980,13 +4983,13 @@
         <v>25</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F134" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H134" s="1" t="s">
         <v>29</v>
@@ -5000,10 +5003,10 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C135" s="1">
         <v>18</v>
@@ -5012,13 +5015,13 @@
         <v>23</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H135" s="1" t="s">
         <v>28</v>
@@ -5032,7 +5035,7 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>10</v>
@@ -5044,16 +5047,16 @@
         <v>39</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F136" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G136" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I136" s="1" t="s">
         <v>20</v>
@@ -5064,7 +5067,7 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>10</v>
@@ -5076,16 +5079,16 @@
         <v>35</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F137" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I137" s="1" t="s">
         <v>20</v>
@@ -5096,7 +5099,7 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>10</v>
@@ -5108,16 +5111,16 @@
         <v>47</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F138" s="1" t="s">
         <v>51</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I138" s="1" t="s">
         <v>20</v>
@@ -5128,7 +5131,7 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>10</v>
@@ -5140,13 +5143,13 @@
         <v>12</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F139" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G139" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H139" s="1" t="s">
         <v>33</v>
@@ -5160,7 +5163,7 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>10</v>
@@ -5172,13 +5175,13 @@
         <v>44</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F140" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G140" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H140" s="1" t="s">
         <v>32</v>
@@ -5192,7 +5195,7 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>10</v>
@@ -5204,16 +5207,16 @@
         <v>19</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F141" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G141" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I141" s="1" t="s">
         <v>14</v>
@@ -5224,7 +5227,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>10</v>
@@ -5236,13 +5239,13 @@
         <v>36</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F142" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H142" s="1" t="s">
         <v>37</v>
@@ -5256,7 +5259,7 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>10</v>
@@ -5268,13 +5271,13 @@
         <v>38</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F143" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H143" s="1" t="s">
         <v>29</v>
@@ -5288,7 +5291,7 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>10</v>
@@ -5300,16 +5303,16 @@
         <v>57</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F144" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>20</v>
@@ -5320,7 +5323,7 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>10</v>
@@ -5332,16 +5335,16 @@
         <v>24</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F145" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I145" s="1" t="s">
         <v>14</v>
@@ -5352,7 +5355,7 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>10</v>
@@ -5364,16 +5367,16 @@
         <v>53</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F146" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I146" s="1" t="s">
         <v>20</v>
@@ -5384,7 +5387,7 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>10</v>
@@ -5396,13 +5399,13 @@
         <v>21</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F147" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H147" s="1" t="s">
         <v>37</v>
@@ -5416,7 +5419,7 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>10</v>
@@ -5425,19 +5428,19 @@
         <v>18</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F148" s="1" t="s">
         <v>48</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>14</v>
@@ -5448,7 +5451,7 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>10</v>
@@ -5460,16 +5463,16 @@
         <v>55</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F149" s="1" t="s">
         <v>50</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I149" s="1" t="s">
         <v>20</v>

</xml_diff>